<commit_message>
Mise à jour de l'envoi des mails
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Info\Random\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personnel\IA\Connerie\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E76A0662-BFC2-4979-A75F-B2F65E5CA245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3DF720-B2A3-4275-B721-7CEDE31783A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6368B415-5513-4B74-987D-85DE16EA6249}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{6368B415-5513-4B74-987D-85DE16EA6249}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -41,28 +30,28 @@
     <t>Nom</t>
   </si>
   <si>
-    <t xml:space="preserve">prénom  </t>
-  </si>
-  <si>
     <t>mail</t>
   </si>
   <si>
     <t>Jean</t>
   </si>
   <si>
-    <t>mahmoud</t>
-  </si>
-  <si>
     <t>washed</t>
   </si>
   <si>
-    <t>only</t>
-  </si>
-  <si>
     <t>antomdr85000@gmail.com</t>
   </si>
   <si>
     <t>niquezebi311@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entreprise  </t>
+  </si>
+  <si>
+    <t>Thales</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
   </si>
 </sst>
 </file>
@@ -428,47 +417,47 @@
   <dimension ref="B3:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
         <v>2</v>
       </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
send only the good Resume to the person
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personnel\IA\Connerie\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Info\Random\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3DF720-B2A3-4275-B721-7CEDE31783A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAF5A15-A2AA-4206-8FDB-CE4F356FDD06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{6368B415-5513-4B74-987D-85DE16EA6249}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6368B415-5513-4B74-987D-85DE16EA6249}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,6 @@
     <t>Jean</t>
   </si>
   <si>
-    <t>washed</t>
-  </si>
-  <si>
-    <t>antomdr85000@gmail.com</t>
-  </si>
-  <si>
     <t>niquezebi311@gmail.com</t>
   </si>
   <si>
@@ -51,7 +45,13 @@
     <t>Thales</t>
   </si>
   <si>
-    <t>Microsoft</t>
+    <t>Leatitia</t>
+  </si>
+  <si>
+    <t>Urban corporation</t>
+  </si>
+  <si>
+    <t>urbain.calt@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -118,9 +118,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -158,7 +158,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -264,7 +264,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -406,7 +406,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -417,47 +417,47 @@
   <dimension ref="B3:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="F5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>